<commit_message>
Version du 26 avril 2022
</commit_message>
<xml_diff>
--- a/resultats/resultats_t1_2022.xlsx
+++ b/resultats/resultats_t1_2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t xml:space="preserve">structure</t>
   </si>
@@ -186,9 +186,6 @@
   </si>
   <si>
     <t xml:space="preserve">Documentation, Diffusion et Archives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Documentation, Diffusion et et Archives</t>
   </si>
   <si>
     <t xml:space="preserve">Imprimerie</t>
@@ -379,8 +376,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:H75" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:H75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:H74" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:H74"/>
   <tableColumns count="8">
     <tableColumn id="1" name="structure"/>
     <tableColumn id="2" name="division"/>
@@ -1839,19 +1836,19 @@
         <v>56</v>
       </c>
       <c r="D10" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E10" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F10" t="n">
-        <v>91.7</v>
+        <v>93.3</v>
       </c>
       <c r="G10" t="n">
         <v>27.3</v>
       </c>
       <c r="H10" t="n">
-        <v>91.7</v>
+        <v>93.3</v>
       </c>
     </row>
     <row r="11">
@@ -1865,19 +1862,19 @@
         <v>57</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G11" t="n">
         <v>27.3</v>
       </c>
       <c r="H11" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -1885,25 +1882,25 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G12" t="n">
         <v>27.3</v>
       </c>
       <c r="H12" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -1914,13 +1911,13 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>100</v>
@@ -1943,10 +1940,10 @@
         <v>59</v>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>100</v>
@@ -1969,10 +1966,10 @@
         <v>60</v>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>100</v>
@@ -1989,25 +1986,25 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
-        <v>100</v>
+        <v>85.7</v>
       </c>
       <c r="G16" t="n">
         <v>27.3</v>
       </c>
       <c r="H16" t="n">
-        <v>100</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="17">
@@ -2018,22 +2015,22 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="D17" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
-        <v>85.7</v>
+        <v>100</v>
       </c>
       <c r="G17" t="n">
         <v>27.3</v>
       </c>
       <c r="H17" t="n">
-        <v>85.7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18">
@@ -2047,19 +2044,19 @@
         <v>62</v>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
-        <v>100</v>
+        <v>85.7</v>
       </c>
       <c r="G18" t="n">
         <v>27.3</v>
       </c>
       <c r="H18" t="n">
-        <v>100</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="19">
@@ -2073,19 +2070,19 @@
         <v>63</v>
       </c>
       <c r="D19" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>85.7</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
         <v>27.3</v>
       </c>
       <c r="H19" t="n">
-        <v>85.7</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="20">
@@ -2093,25 +2090,25 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>85.7</v>
       </c>
       <c r="G20" t="n">
         <v>27.3</v>
       </c>
       <c r="H20" t="n">
-        <v>27.3</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="21">
@@ -2122,22 +2119,22 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D21" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
-        <v>85.7</v>
+        <v>100</v>
       </c>
       <c r="G21" t="n">
         <v>27.3</v>
       </c>
       <c r="H21" t="n">
-        <v>85.7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22">
@@ -2151,10 +2148,10 @@
         <v>59</v>
       </c>
       <c r="D22" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>100</v>
@@ -2177,10 +2174,10 @@
         <v>60</v>
       </c>
       <c r="D23" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>100</v>
@@ -2197,25 +2194,25 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="D24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E24" t="n">
         <v>2</v>
       </c>
       <c r="F24" t="n">
-        <v>100</v>
+        <v>66.7</v>
       </c>
       <c r="G24" t="n">
         <v>27.3</v>
       </c>
       <c r="H24" t="n">
-        <v>100</v>
+        <v>66.7</v>
       </c>
     </row>
     <row r="25">
@@ -2226,22 +2223,22 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D25" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
-        <v>66.7</v>
+        <v>100</v>
       </c>
       <c r="G25" t="n">
         <v>27.3</v>
       </c>
       <c r="H25" t="n">
-        <v>66.7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26">
@@ -2252,7 +2249,7 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D26" t="n">
         <v>7</v>
@@ -2275,16 +2272,16 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D27" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>100</v>
@@ -2304,13 +2301,13 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D28" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>100</v>
@@ -2333,10 +2330,10 @@
         <v>59</v>
       </c>
       <c r="D29" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>100</v>
@@ -2353,25 +2350,25 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="D30" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G30" t="n">
         <v>27.3</v>
       </c>
       <c r="H30" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31">
@@ -2382,22 +2379,22 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D31" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F31" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="G31" t="n">
         <v>27.3</v>
       </c>
       <c r="H31" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32">
@@ -2411,10 +2408,10 @@
         <v>59</v>
       </c>
       <c r="D32" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E32" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>100</v>
@@ -2431,16 +2428,16 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D33" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>100</v>
@@ -2460,22 +2457,22 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D34" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
-        <v>100</v>
+        <v>85.7</v>
       </c>
       <c r="G34" t="n">
         <v>27.3</v>
       </c>
       <c r="H34" t="n">
-        <v>100</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="35">
@@ -2489,19 +2486,19 @@
         <v>59</v>
       </c>
       <c r="D35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E35" t="n">
         <v>6</v>
       </c>
       <c r="F35" t="n">
-        <v>85.7</v>
+        <v>100</v>
       </c>
       <c r="G35" t="n">
         <v>27.3</v>
       </c>
       <c r="H35" t="n">
-        <v>85.7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36">
@@ -2515,10 +2512,10 @@
         <v>60</v>
       </c>
       <c r="D36" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F36" t="n">
         <v>100</v>
@@ -2535,16 +2532,16 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>100</v>
@@ -2564,13 +2561,13 @@
         <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D38" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
         <v>100</v>
@@ -2593,10 +2590,10 @@
         <v>59</v>
       </c>
       <c r="D39" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>100</v>
@@ -2619,10 +2616,10 @@
         <v>60</v>
       </c>
       <c r="D40" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>100</v>
@@ -2639,51 +2636,51 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G41" t="n">
         <v>27.3</v>
       </c>
       <c r="H41" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C42" t="s">
         <v>66</v>
       </c>
       <c r="D42" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F42" t="n">
-        <v>60</v>
+        <v>82.6</v>
       </c>
       <c r="G42" t="n">
-        <v>27.3</v>
+        <v>37.5</v>
       </c>
       <c r="H42" t="n">
-        <v>60</v>
+        <v>82.6</v>
       </c>
     </row>
     <row r="43">
@@ -2697,19 +2694,19 @@
         <v>67</v>
       </c>
       <c r="D43" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E43" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
-        <v>82.6</v>
+        <v>88.9</v>
       </c>
       <c r="G43" t="n">
         <v>37.5</v>
       </c>
       <c r="H43" t="n">
-        <v>82.6</v>
+        <v>88.9</v>
       </c>
     </row>
     <row r="44">
@@ -2717,25 +2714,25 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C44" t="s">
         <v>68</v>
       </c>
       <c r="D44" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E44" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F44" t="n">
-        <v>88.9</v>
+        <v>92.6</v>
       </c>
       <c r="G44" t="n">
         <v>37.5</v>
       </c>
       <c r="H44" t="n">
-        <v>88.9</v>
+        <v>92.6</v>
       </c>
     </row>
     <row r="45">
@@ -2749,19 +2746,19 @@
         <v>69</v>
       </c>
       <c r="D45" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E45" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F45" t="n">
-        <v>92.6</v>
+        <v>87</v>
       </c>
       <c r="G45" t="n">
         <v>37.5</v>
       </c>
       <c r="H45" t="n">
-        <v>92.6</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46">
@@ -2769,25 +2766,25 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
         <v>70</v>
       </c>
       <c r="D46" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E46" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F46" t="n">
-        <v>87</v>
+        <v>85.7</v>
       </c>
       <c r="G46" t="n">
         <v>37.5</v>
       </c>
       <c r="H46" t="n">
-        <v>87</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="47">
@@ -2801,19 +2798,19 @@
         <v>71</v>
       </c>
       <c r="D47" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E47" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
-        <v>85.7</v>
+        <v>37.5</v>
       </c>
       <c r="G47" t="n">
         <v>37.5</v>
       </c>
       <c r="H47" t="n">
-        <v>85.7</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="48">
@@ -2827,42 +2824,42 @@
         <v>72</v>
       </c>
       <c r="D48" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
-        <v>37.5</v>
+        <v>100</v>
       </c>
       <c r="G48" t="n">
         <v>37.5</v>
       </c>
       <c r="H48" t="n">
-        <v>37.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C49" t="s">
         <v>73</v>
       </c>
       <c r="D49" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
         <v>100</v>
       </c>
       <c r="G49" t="n">
-        <v>37.5</v>
+        <v>100</v>
       </c>
       <c r="H49" t="n">
         <v>100</v>
@@ -2879,10 +2876,10 @@
         <v>74</v>
       </c>
       <c r="D50" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>100</v>
@@ -2905,10 +2902,10 @@
         <v>75</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>100</v>
@@ -2922,19 +2919,19 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s">
         <v>76</v>
       </c>
       <c r="D52" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>100</v>
@@ -2957,10 +2954,10 @@
         <v>77</v>
       </c>
       <c r="D53" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F53" t="n">
         <v>100</v>
@@ -2983,10 +2980,10 @@
         <v>78</v>
       </c>
       <c r="D54" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E54" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>100</v>
@@ -3009,10 +3006,10 @@
         <v>79</v>
       </c>
       <c r="D55" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>100</v>
@@ -3026,28 +3023,28 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C56" t="s">
         <v>80</v>
       </c>
       <c r="D56" t="n">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F56" t="n">
-        <v>100</v>
+        <v>22.4</v>
       </c>
       <c r="G56" t="n">
-        <v>100</v>
+        <v>12.5</v>
       </c>
       <c r="H56" t="n">
-        <v>100</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="57">
@@ -3055,25 +3052,25 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s">
         <v>81</v>
       </c>
       <c r="D57" t="n">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="E57" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
-        <v>22.4</v>
+        <v>80</v>
       </c>
       <c r="G57" t="n">
         <v>12.5</v>
       </c>
       <c r="H57" t="n">
-        <v>22.4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58">
@@ -3087,19 +3084,19 @@
         <v>82</v>
       </c>
       <c r="D58" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
-        <v>80</v>
+        <v>12.5</v>
       </c>
       <c r="G58" t="n">
         <v>12.5</v>
       </c>
       <c r="H58" t="n">
-        <v>80</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="59">
@@ -3107,25 +3104,25 @@
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C59" t="s">
         <v>83</v>
       </c>
       <c r="D59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
-        <v>12.5</v>
+        <v>42.9</v>
       </c>
       <c r="G59" t="n">
         <v>12.5</v>
       </c>
       <c r="H59" t="n">
-        <v>12.5</v>
+        <v>42.9</v>
       </c>
     </row>
     <row r="60">
@@ -3142,42 +3139,42 @@
         <v>7</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
-        <v>42.9</v>
+        <v>57.1</v>
       </c>
       <c r="G60" t="n">
         <v>12.5</v>
       </c>
       <c r="H60" t="n">
-        <v>42.9</v>
+        <v>57.1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C61" t="s">
         <v>85</v>
       </c>
       <c r="D61" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F61" t="n">
-        <v>57.1</v>
+        <v>96.8</v>
       </c>
       <c r="G61" t="n">
-        <v>12.5</v>
+        <v>75</v>
       </c>
       <c r="H61" t="n">
-        <v>57.1</v>
+        <v>96.8</v>
       </c>
     </row>
     <row r="62">
@@ -3185,25 +3182,25 @@
         <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C62" t="s">
         <v>86</v>
       </c>
       <c r="D62" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E62" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F62" t="n">
-        <v>96.8</v>
+        <v>87.5</v>
       </c>
       <c r="G62" t="n">
         <v>75</v>
       </c>
       <c r="H62" t="n">
-        <v>96.8</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="63">
@@ -3217,45 +3214,45 @@
         <v>87</v>
       </c>
       <c r="D63" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E63" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
-        <v>87.5</v>
+        <v>75</v>
       </c>
       <c r="G63" t="n">
         <v>75</v>
       </c>
       <c r="H63" t="n">
-        <v>87.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C64" t="s">
         <v>88</v>
       </c>
       <c r="D64" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="G64" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H64" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65">
@@ -3272,16 +3269,16 @@
         <v>1</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G65" t="n">
         <v>80</v>
       </c>
       <c r="H65" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66">
@@ -3289,19 +3286,19 @@
         <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C66" t="s">
         <v>90</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G66" t="n">
         <v>80</v>
@@ -3321,19 +3318,19 @@
         <v>91</v>
       </c>
       <c r="D67" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G67" t="n">
         <v>80</v>
       </c>
       <c r="H67" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68">
@@ -3341,7 +3338,7 @@
         <v>14</v>
       </c>
       <c r="B68" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C68" t="s">
         <v>92</v>
@@ -3373,10 +3370,10 @@
         <v>93</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>100</v>
@@ -3390,28 +3387,26 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>15</v>
+      </c>
+      <c r="B70" t="s">
+        <v>47</v>
+      </c>
+      <c r="C70"/>
+      <c r="D70" t="n">
         <v>14</v>
       </c>
-      <c r="B70" t="s">
-        <v>46</v>
-      </c>
-      <c r="C70" t="s">
-        <v>94</v>
-      </c>
-      <c r="D70" t="n">
-        <v>6</v>
-      </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F70" t="n">
-        <v>100</v>
+        <v>92.9</v>
       </c>
       <c r="G70" t="n">
-        <v>80</v>
+        <v>87.5</v>
       </c>
       <c r="H70" t="n">
-        <v>100</v>
+        <v>92.9</v>
       </c>
     </row>
     <row r="71">
@@ -3419,23 +3414,23 @@
         <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C71"/>
       <c r="D71" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E71" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
-        <v>92.9</v>
+        <v>100</v>
       </c>
       <c r="G71" t="n">
         <v>87.5</v>
       </c>
       <c r="H71" t="n">
-        <v>92.9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72">
@@ -3443,94 +3438,70 @@
         <v>15</v>
       </c>
       <c r="B72" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C72"/>
       <c r="D72" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
-        <v>100</v>
+        <v>87.5</v>
       </c>
       <c r="G72" t="n">
         <v>87.5</v>
       </c>
       <c r="H72" t="n">
-        <v>100</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>15</v>
-      </c>
-      <c r="B73" t="s">
-        <v>48</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B73"/>
       <c r="C73"/>
       <c r="D73" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
-        <v>87.5</v>
+        <v>60</v>
       </c>
       <c r="G73" t="n">
-        <v>87.5</v>
+        <v>60</v>
       </c>
       <c r="H73" t="n">
-        <v>87.5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>16</v>
-      </c>
-      <c r="B74"/>
-      <c r="C74"/>
+        <v>17</v>
+      </c>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" t="s">
+        <v>17</v>
+      </c>
       <c r="D74" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G74" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="H74" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>17</v>
-      </c>
-      <c r="B75" t="s">
-        <v>17</v>
-      </c>
-      <c r="C75" t="s">
-        <v>17</v>
-      </c>
-      <c r="D75" t="n">
-        <v>8</v>
-      </c>
-      <c r="E75" t="n">
-        <v>8</v>
-      </c>
-      <c r="F75" t="n">
-        <v>100</v>
-      </c>
-      <c r="G75" t="n">
-        <v>100</v>
-      </c>
-      <c r="H75" t="n">
         <v>100</v>
       </c>
     </row>
@@ -3553,7 +3524,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>

</xml_diff>